<commit_message>
Gave the valid name to the activities and implemented the concept for no jobs found
</commit_message>
<xml_diff>
--- a/Data/Input/Job-Seekers-List.xlsx
+++ b/Data/Input/Job-Seekers-List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>No.</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Sasireka</t>
+  </si>
+  <si>
+    <t>Technical Manager</t>
+  </si>
+  <si>
+    <t>Solution</t>
   </si>
 </sst>
 </file>
@@ -410,7 +416,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,7 +452,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -474,7 +480,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -488,7 +494,7 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -502,7 +508,7 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>